<commit_message>
Hopefully solved cumulative_voting, aggregating with product.
</commit_message>
<xml_diff>
--- a/results/approved_voters=10_projects=15.xlsx
+++ b/results/approved_voters=10_projects=15.xlsx
@@ -1,138 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
-  <si>
-    <t>project0</t>
-  </si>
-  <si>
-    <t>project1</t>
-  </si>
-  <si>
-    <t>project2</t>
-  </si>
-  <si>
-    <t>project3</t>
-  </si>
-  <si>
-    <t>project4</t>
-  </si>
-  <si>
-    <t>project5</t>
-  </si>
-  <si>
-    <t>project6</t>
-  </si>
-  <si>
-    <t>project7</t>
-  </si>
-  <si>
-    <t>project8</t>
-  </si>
-  <si>
-    <t>project9</t>
-  </si>
-  <si>
-    <t>project10</t>
-  </si>
-  <si>
-    <t>project11</t>
-  </si>
-  <si>
-    <t>project12</t>
-  </si>
-  <si>
-    <t>project13</t>
-  </si>
-  <si>
-    <t>project14</t>
-  </si>
-  <si>
-    <t>approval</t>
-  </si>
-  <si>
-    <t>threshold</t>
-  </si>
-  <si>
-    <t>utility sum</t>
-  </si>
-  <si>
-    <t>utility ratio</t>
-  </si>
-  <si>
-    <t>utility product</t>
-  </si>
-  <si>
-    <t>cumulative sum</t>
-  </si>
-  <si>
-    <t>cumulative ratio</t>
-  </si>
-  <si>
-    <t>cumulative product</t>
-  </si>
-  <si>
-    <t>knapsack</t>
-  </si>
-  <si>
-    <t>knapsack ratio</t>
-  </si>
-  <si>
-    <t>default borda</t>
-  </si>
-  <si>
-    <t>default borda truncated</t>
-  </si>
-  <si>
-    <t>dowdall system borda</t>
-  </si>
-  <si>
-    <t>dowdall system borda truncated</t>
-  </si>
-  <si>
-    <t>eurovision song contest borda</t>
-  </si>
-  <si>
-    <t>eurovision song contest borda truncated</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -147,35 +46,94 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -463,96 +421,134 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:16">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16">
-      <c r="A2" s="1" t="s">
-        <v>15</v>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>project0</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>project1</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>project2</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>project3</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>project4</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>project5</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>project6</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>project7</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>project8</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>project9</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>project10</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>project11</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>project12</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>project13</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>project14</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>approval</t>
+        </is>
       </c>
       <c r="B2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
       </c>
       <c r="D2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2" t="b">
         <v>0</v>
       </c>
       <c r="H2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K2" t="b">
         <v>1</v>
       </c>
       <c r="L2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M2" t="b">
         <v>1</v>
@@ -564,18 +560,20 @@
         <v>0</v>
       </c>
       <c r="P2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
-      <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>threshold</t>
+        </is>
       </c>
       <c r="B3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
@@ -587,39 +585,46 @@
         <v>0</v>
       </c>
       <c r="G3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3" t="b">
         <v>1</v>
       </c>
       <c r="I3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:16">
-      <c r="A4" s="1" t="s">
-        <v>17</v>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>utility sum</t>
+        </is>
       </c>
       <c r="B4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" t="b">
         <v>0</v>
       </c>
       <c r="E4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4" t="b">
         <v>1</v>
@@ -628,16 +633,16 @@
         <v>1</v>
       </c>
       <c r="I4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4" t="b">
         <v>1</v>
       </c>
       <c r="L4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M4" t="b">
         <v>1</v>
@@ -649,27 +654,29 @@
         <v>0</v>
       </c>
       <c r="P4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16">
-      <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>utility ratio</t>
+        </is>
       </c>
       <c r="B5" t="b">
         <v>1</v>
       </c>
       <c r="C5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" t="b">
         <v>1</v>
@@ -681,13 +688,13 @@
         <v>1</v>
       </c>
       <c r="J5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M5" t="b">
         <v>1</v>
@@ -699,18 +706,20 @@
         <v>0</v>
       </c>
       <c r="P5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16">
-      <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>utility product</t>
+        </is>
       </c>
       <c r="B6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" t="b">
         <v>0</v>
@@ -719,7 +728,7 @@
         <v>0</v>
       </c>
       <c r="F6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" t="b">
         <v>1</v>
@@ -728,7 +737,7 @@
         <v>1</v>
       </c>
       <c r="I6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6" t="b">
         <v>1</v>
@@ -737,7 +746,7 @@
         <v>1</v>
       </c>
       <c r="L6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M6" t="b">
         <v>1</v>
@@ -749,27 +758,29 @@
         <v>0</v>
       </c>
       <c r="P6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16">
-      <c r="A7" s="1" t="s">
-        <v>20</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>cumulative sum</t>
+        </is>
       </c>
       <c r="B7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" t="b">
         <v>0</v>
       </c>
       <c r="E7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" t="b">
         <v>1</v>
@@ -778,16 +789,16 @@
         <v>1</v>
       </c>
       <c r="I7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K7" t="b">
         <v>1</v>
       </c>
       <c r="L7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M7" t="b">
         <v>1</v>
@@ -799,18 +810,20 @@
         <v>0</v>
       </c>
       <c r="P7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16">
-      <c r="A8" s="1" t="s">
-        <v>21</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>cumulative ratio</t>
+        </is>
       </c>
       <c r="B8" t="b">
         <v>1</v>
       </c>
       <c r="C8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" t="b">
         <v>0</v>
@@ -819,7 +832,7 @@
         <v>1</v>
       </c>
       <c r="F8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" t="b">
         <v>1</v>
@@ -834,7 +847,7 @@
         <v>1</v>
       </c>
       <c r="K8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L8" t="b">
         <v>0</v>
@@ -849,18 +862,20 @@
         <v>0</v>
       </c>
       <c r="P8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16">
-      <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>cumulative product</t>
+        </is>
       </c>
       <c r="B9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" t="b">
         <v>0</v>
@@ -869,7 +884,7 @@
         <v>0</v>
       </c>
       <c r="F9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" t="b">
         <v>1</v>
@@ -878,7 +893,7 @@
         <v>1</v>
       </c>
       <c r="I9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9" t="b">
         <v>1</v>
@@ -887,7 +902,7 @@
         <v>1</v>
       </c>
       <c r="L9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M9" t="b">
         <v>1</v>
@@ -899,12 +914,14 @@
         <v>0</v>
       </c>
       <c r="P9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16">
-      <c r="A10" s="1" t="s">
-        <v>23</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>knapsack</t>
+        </is>
       </c>
       <c r="B10" t="b">
         <v>0</v>
@@ -931,15 +948,22 @@
         <v>1</v>
       </c>
       <c r="J10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:16">
-      <c r="A11" s="1" t="s">
-        <v>24</v>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>knapsack ratio</t>
+        </is>
       </c>
       <c r="B11" t="b">
         <v>0</v>
@@ -960,7 +984,7 @@
         <v>1</v>
       </c>
       <c r="H11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I11" t="b">
         <v>1</v>
@@ -969,27 +993,34 @@
         <v>1</v>
       </c>
       <c r="K11" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16">
-      <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>0</v>
+      </c>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
+      <c r="P11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>default borda</t>
+        </is>
       </c>
       <c r="B12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" t="b">
         <v>0</v>
       </c>
       <c r="E12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" t="b">
         <v>1</v>
@@ -998,16 +1029,16 @@
         <v>1</v>
       </c>
       <c r="I12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K12" t="b">
         <v>1</v>
       </c>
       <c r="L12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M12" t="b">
         <v>1</v>
@@ -1019,45 +1050,47 @@
         <v>0</v>
       </c>
       <c r="P12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16">
-      <c r="A13" s="1" t="s">
-        <v>26</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>default borda truncated</t>
+        </is>
       </c>
       <c r="B13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" t="b">
         <v>1</v>
       </c>
       <c r="D13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" t="b">
         <v>1</v>
       </c>
       <c r="F13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I13" t="b">
         <v>0</v>
       </c>
       <c r="J13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K13" t="b">
         <v>1</v>
       </c>
       <c r="L13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M13" t="b">
         <v>1</v>
@@ -1072,15 +1105,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
-      <c r="A14" s="1" t="s">
-        <v>27</v>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>dowdall system borda</t>
+        </is>
       </c>
       <c r="B14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" t="b">
         <v>0</v>
@@ -1089,22 +1124,22 @@
         <v>1</v>
       </c>
       <c r="F14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" t="b">
         <v>1</v>
       </c>
       <c r="H14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" t="b">
         <v>1</v>
       </c>
       <c r="K14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L14" t="b">
         <v>1</v>
@@ -1119,18 +1154,20 @@
         <v>0</v>
       </c>
       <c r="P14" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16">
-      <c r="A15" s="1" t="s">
-        <v>28</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>dowdall system borda truncated</t>
+        </is>
       </c>
       <c r="B15" t="b">
         <v>1</v>
       </c>
       <c r="C15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" t="b">
         <v>0</v>
@@ -1139,13 +1176,13 @@
         <v>1</v>
       </c>
       <c r="F15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15" t="b">
         <v>1</v>
       </c>
       <c r="H15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I15" t="b">
         <v>0</v>
@@ -1154,7 +1191,7 @@
         <v>1</v>
       </c>
       <c r="K15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L15" t="b">
         <v>1</v>
@@ -1172,15 +1209,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
-      <c r="A16" s="1" t="s">
-        <v>29</v>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>eurovision song contest borda</t>
+        </is>
       </c>
       <c r="B16" t="b">
         <v>1</v>
       </c>
       <c r="C16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" t="b">
         <v>0</v>
@@ -1189,13 +1228,13 @@
         <v>1</v>
       </c>
       <c r="F16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I16" t="b">
         <v>0</v>
@@ -1207,7 +1246,7 @@
         <v>1</v>
       </c>
       <c r="L16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M16" t="b">
         <v>1</v>
@@ -1219,12 +1258,14 @@
         <v>0</v>
       </c>
       <c r="P16" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16">
-      <c r="A17" s="1" t="s">
-        <v>30</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>eurovision song contest borda truncated</t>
+        </is>
       </c>
       <c r="B17" t="b">
         <v>1</v>
@@ -1239,25 +1280,25 @@
         <v>1</v>
       </c>
       <c r="F17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17" t="b">
         <v>1</v>
       </c>
       <c r="H17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I17" t="b">
         <v>0</v>
       </c>
       <c r="J17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K17" t="b">
         <v>1</v>
       </c>
       <c r="L17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M17" t="b">
         <v>1</v>
@@ -1273,6 +1314,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>